<commit_message>
[fix] create computer fixed
</commit_message>
<xml_diff>
--- a/input_glpi.xlsx
+++ b/input_glpi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OneDriveFalse\1 - KevDev\2 - Estudos\Testes de codigo\GLPI scripts\Input de informações e criação de coisas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302A548A-9C8C-4A27-861E-CC7F144009BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2478A3F-1DB1-482F-AD0A-B22574EFD1A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="1968" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GLPI Input" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="91">
   <si>
     <t>Nome do User</t>
   </si>
@@ -65,9 +65,6 @@
     <t>João Silva</t>
   </si>
   <si>
-    <t>Time1</t>
-  </si>
-  <si>
     <t>551199999999</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>Pedro Oliveira</t>
   </si>
   <si>
-    <t>Suporte</t>
-  </si>
-  <si>
     <t>551198888777</t>
   </si>
   <si>
@@ -113,15 +107,9 @@
     <t>Ana Santos</t>
   </si>
   <si>
-    <t>Financeiro</t>
-  </si>
-  <si>
     <t>Lucas Pereira</t>
   </si>
   <si>
-    <t>Vendas</t>
-  </si>
-  <si>
     <t>551197777666</t>
   </si>
   <si>
@@ -137,9 +125,6 @@
     <t>Rafael Costa</t>
   </si>
   <si>
-    <t>RH</t>
-  </si>
-  <si>
     <t>Acer</t>
   </si>
   <si>
@@ -170,9 +155,6 @@
     <t>Camila Rodrigues</t>
   </si>
   <si>
-    <t>Marketing</t>
-  </si>
-  <si>
     <t>551195555444</t>
   </si>
   <si>
@@ -300,13 +282,37 @@
   </si>
   <si>
     <t>Vivo</t>
+  </si>
+  <si>
+    <t>Cr@email.com</t>
+  </si>
+  <si>
+    <t>Volkswagen</t>
+  </si>
+  <si>
+    <t>Saint Gobain</t>
+  </si>
+  <si>
+    <t>Promotor</t>
+  </si>
+  <si>
+    <t>Tecnico</t>
+  </si>
+  <si>
+    <t>Solution Center</t>
+  </si>
+  <si>
+    <t>Gomes da Costa</t>
+  </si>
+  <si>
+    <t>Tipo de computador</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,6 +322,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -344,14 +358,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -652,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,25 +681,27 @@
     <col min="2" max="3" width="16.42578125" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="13.140625" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20" customWidth="1"/>
-    <col min="14" max="14" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20" customWidth="1"/>
+    <col min="15" max="15" width="27" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -694,374 +713,419 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="M1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>79</v>
+      <c r="Q1" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C2">
         <v>35686234657</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
-        <v>87</v>
-      </c>
-      <c r="I2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>12</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>13</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
+        <v>58</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
         <v>14</v>
       </c>
-      <c r="M2" t="s">
-        <v>64</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="Q2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="O2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C3">
         <v>35686234658</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
-      </c>
-      <c r="L3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" t="s">
+        <v>59</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
         <v>17</v>
       </c>
-      <c r="M3" t="s">
-        <v>65</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="Q3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="O3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C4">
         <v>35686234659</v>
       </c>
       <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" t="s">
+        <v>70</v>
+      </c>
+      <c r="L4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" t="s">
+        <v>60</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
         <v>48</v>
-      </c>
-      <c r="E4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s">
-        <v>88</v>
-      </c>
-      <c r="I4" t="s">
-        <v>71</v>
-      </c>
-      <c r="J4" t="s">
-        <v>76</v>
-      </c>
-      <c r="K4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" t="s">
-        <v>23</v>
-      </c>
-      <c r="M4" t="s">
-        <v>66</v>
-      </c>
-      <c r="N4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>54</v>
       </c>
       <c r="C5">
         <v>35686234660</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>85</v>
+      </c>
+      <c r="G5" t="s">
+        <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C6">
         <v>35686234661</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="H6" t="s">
-        <v>88</v>
+        <v>25</v>
       </c>
       <c r="I6" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="J6" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="K6" t="s">
-        <v>30</v>
+        <v>69</v>
+      </c>
+      <c r="L6" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C7">
         <v>35686234662</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
-      </c>
-      <c r="L7" t="s">
-        <v>14</v>
+        <v>54</v>
+      </c>
+      <c r="F7" t="s">
+        <v>89</v>
       </c>
       <c r="M7" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="N7" t="s">
-        <v>32</v>
-      </c>
-      <c r="O7" t="s">
-        <v>83</v>
+        <v>61</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+      <c r="P7" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C8">
         <v>35686234663</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" t="s">
+        <v>65</v>
+      </c>
+      <c r="M8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N8" t="s">
         <v>62</v>
       </c>
-      <c r="F8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L8" t="s">
-        <v>35</v>
-      </c>
-      <c r="M8" t="s">
-        <v>68</v>
-      </c>
-      <c r="N8" t="s">
-        <v>36</v>
-      </c>
-      <c r="O8" t="s">
-        <v>84</v>
+      <c r="O8">
+        <v>2</v>
+      </c>
+      <c r="P8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C9">
         <v>35686234664</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" t="s">
-        <v>38</v>
+        <v>56</v>
+      </c>
+      <c r="F9" t="s">
+        <v>65</v>
       </c>
       <c r="H9" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="I9" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="J9" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="K9" t="s">
-        <v>40</v>
+        <v>34</v>
+      </c>
+      <c r="L9" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C10">
         <v>35686234665</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" t="s">
+        <v>37</v>
+      </c>
+      <c r="M10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N10" t="s">
         <v>63</v>
       </c>
-      <c r="F10" t="s">
-        <v>42</v>
-      </c>
-      <c r="L10" t="s">
-        <v>17</v>
-      </c>
-      <c r="M10" t="s">
-        <v>69</v>
-      </c>
-      <c r="N10" t="s">
-        <v>43</v>
-      </c>
-      <c r="O10" t="s">
-        <v>85</v>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" t="s">
-        <v>56</v>
+        <v>39</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="C11">
         <v>35686234666</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="H11" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="I11" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="J11" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="K11" t="s">
-        <v>47</v>
+        <v>68</v>
+      </c>
+      <c r="L11" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B11" r:id="rId1" xr:uid="{A666A66F-87FA-46AB-96C6-68D6501B3CE2}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[update] create users updated
</commit_message>
<xml_diff>
--- a/input_glpi.xlsx
+++ b/input_glpi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OneDriveFalse\1 - KevDev\2 - Estudos\Testes de codigo\GLPI scripts\Input de informações e criação de coisas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A68E525-D025-43CB-9F5A-3F96784A29AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E6DFFC-F0BD-4FFF-949E-9410AFECD50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="109">
   <si>
     <t>Nome do User</t>
   </si>
@@ -342,6 +342,24 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Tipo de celular</t>
+  </si>
+  <si>
+    <t>Comentario Celular</t>
+  </si>
+  <si>
+    <t>teste</t>
+  </si>
+  <si>
+    <t>Comentario note</t>
+  </si>
+  <si>
+    <t>testeee</t>
+  </si>
+  <si>
+    <t>Status User</t>
   </si>
 </sst>
 </file>
@@ -707,36 +725,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V11"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
-    <col min="10" max="11" width="13.140625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20" customWidth="1"/>
-    <col min="17" max="17" width="27" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="11" max="13" width="13.140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" style="3" customWidth="1"/>
+    <col min="18" max="18" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="20" customWidth="1"/>
-    <col min="20" max="20" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20" customWidth="1"/>
+    <col min="23" max="23" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -746,65 +766,77 @@
       <c r="C1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
+      <c r="D1" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>93</v>
       </c>
+      <c r="Z1" s="4" t="s">
+        <v>106</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -814,62 +846,74 @@
       <c r="C2">
         <v>35686234657</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>42</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>55</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>84</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="3">
-        <v>1</v>
-      </c>
       <c r="K2" s="3">
+        <v>1</v>
+      </c>
+      <c r="L2" s="3">
         <v>3</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" s="3">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
         <v>64</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>11</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>12</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" t="s">
         <v>13</v>
       </c>
-      <c r="P2" t="s">
+      <c r="S2" t="s">
         <v>58</v>
       </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
         <v>14</v>
       </c>
-      <c r="S2" t="s">
+      <c r="V2" t="s">
         <v>74</v>
       </c>
-      <c r="T2" t="s">
+      <c r="W2" t="s">
         <v>94</v>
       </c>
-      <c r="U2" t="s">
+      <c r="X2" t="s">
         <v>97</v>
       </c>
-      <c r="V2" t="s">
+      <c r="Y2" t="s">
         <v>100</v>
       </c>
+      <c r="Z2" s="3" t="s">
+        <v>107</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -879,41 +923,47 @@
       <c r="C3">
         <v>35686234658</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>42</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>55</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>84</v>
       </c>
-      <c r="O3" t="s">
+      <c r="R3" t="s">
         <v>16</v>
       </c>
-      <c r="P3" t="s">
+      <c r="S3" t="s">
         <v>59</v>
       </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-      <c r="R3" t="s">
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3" t="s">
         <v>17</v>
       </c>
-      <c r="S3" t="s">
+      <c r="V3" t="s">
         <v>75</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>100</v>
       </c>
+      <c r="Z3" s="3" t="s">
+        <v>107</v>
+      </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -923,65 +973,75 @@
       <c r="C4">
         <v>35686234659</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
         <v>42</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>54</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>85</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>86</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>19</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>82</v>
       </c>
-      <c r="J4" s="3">
+      <c r="K4" s="3">
         <v>2</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L4" s="3">
         <v>3</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" s="3">
+        <v>2</v>
+      </c>
+      <c r="N4" t="s">
         <v>65</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>70</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>20</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Q4" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="R4" t="s">
         <v>21</v>
       </c>
-      <c r="P4" t="s">
+      <c r="S4" t="s">
         <v>60</v>
       </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-      <c r="R4" t="s">
+      <c r="T4">
+        <v>1</v>
+      </c>
+      <c r="U4" t="s">
         <v>22</v>
       </c>
-      <c r="S4" t="s">
+      <c r="V4" t="s">
         <v>76</v>
       </c>
-      <c r="T4" t="s">
+      <c r="W4" t="s">
         <v>95</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="X4" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>99</v>
       </c>
+      <c r="Z4" s="3"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -991,20 +1051,24 @@
       <c r="C5">
         <v>35686234660</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
         <v>42</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>54</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>85</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>87</v>
       </c>
+      <c r="Z5" s="3"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1014,41 +1078,48 @@
       <c r="C6">
         <v>35686234661</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
         <v>42</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>54</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>85</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>86</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>25</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>82</v>
       </c>
-      <c r="J6" s="3">
-        <v>1</v>
-      </c>
       <c r="K6" s="3">
+        <v>1</v>
+      </c>
+      <c r="L6" s="3">
         <v>3</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" s="3">
+        <v>1</v>
+      </c>
+      <c r="N6" t="s">
         <v>66</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>69</v>
       </c>
-      <c r="N6" t="s">
+      <c r="P6" t="s">
         <v>26</v>
       </c>
+      <c r="Z6" s="3"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1058,41 +1129,47 @@
       <c r="C7">
         <v>35686234662</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
         <v>42</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>54</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>89</v>
       </c>
-      <c r="O7" t="s">
+      <c r="R7" t="s">
         <v>13</v>
       </c>
-      <c r="P7" t="s">
+      <c r="S7" t="s">
         <v>61</v>
       </c>
-      <c r="Q7">
+      <c r="T7">
         <v>2</v>
       </c>
-      <c r="R7" t="s">
+      <c r="U7" t="s">
         <v>28</v>
       </c>
-      <c r="S7" t="s">
+      <c r="V7" t="s">
         <v>77</v>
       </c>
-      <c r="T7" s="3" t="s">
+      <c r="W7" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="U7" t="s">
+      <c r="X7" t="s">
         <v>98</v>
       </c>
-      <c r="V7" t="s">
+      <c r="Y7" t="s">
         <v>99</v>
       </c>
+      <c r="Z7" s="3" t="s">
+        <v>105</v>
+      </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1102,41 +1179,45 @@
       <c r="C8">
         <v>35686234663</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
         <v>42</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>56</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>65</v>
       </c>
-      <c r="O8" t="s">
+      <c r="R8" t="s">
         <v>30</v>
       </c>
-      <c r="P8" t="s">
+      <c r="S8" t="s">
         <v>62</v>
       </c>
-      <c r="Q8">
+      <c r="T8">
         <v>2</v>
       </c>
-      <c r="R8" t="s">
+      <c r="U8" t="s">
         <v>31</v>
       </c>
-      <c r="S8" t="s">
+      <c r="V8" t="s">
         <v>78</v>
       </c>
-      <c r="T8" s="3" t="s">
+      <c r="W8" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="U8" s="3" t="s">
+      <c r="X8" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="V8" s="3" t="s">
+      <c r="Y8" s="3" t="s">
         <v>99</v>
       </c>
+      <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1146,38 +1227,45 @@
       <c r="C9">
         <v>35686234664</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
         <v>42</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>56</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>65</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>33</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>82</v>
       </c>
-      <c r="J9" s="3">
+      <c r="K9" s="3">
         <v>2</v>
       </c>
-      <c r="K9" s="3">
+      <c r="L9" s="3">
         <v>5</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" s="3">
+        <v>1</v>
+      </c>
+      <c r="N9" t="s">
         <v>64</v>
       </c>
-      <c r="M9" t="s">
+      <c r="O9" t="s">
         <v>34</v>
       </c>
-      <c r="N9" t="s">
+      <c r="P9" t="s">
         <v>35</v>
       </c>
+      <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1187,41 +1275,45 @@
       <c r="C10">
         <v>35686234665</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
         <v>42</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>57</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>37</v>
       </c>
-      <c r="O10" t="s">
+      <c r="R10" t="s">
         <v>16</v>
       </c>
-      <c r="P10" t="s">
+      <c r="S10" t="s">
         <v>63</v>
       </c>
-      <c r="Q10">
-        <v>1</v>
-      </c>
-      <c r="R10" t="s">
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10" t="s">
         <v>38</v>
       </c>
-      <c r="S10" t="s">
+      <c r="V10" t="s">
         <v>79</v>
       </c>
-      <c r="T10" s="3" t="s">
+      <c r="W10" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="U10" s="3" t="s">
+      <c r="X10" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="V10" t="s">
+      <c r="Y10" t="s">
         <v>99</v>
       </c>
+      <c r="Z10" s="3"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1231,34 +1323,40 @@
       <c r="C11">
         <v>35686234666</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
         <v>42</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>57</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>88</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>40</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>81</v>
       </c>
-      <c r="J11" s="3">
+      <c r="K11" s="3">
         <v>3</v>
       </c>
-      <c r="K11" s="3">
+      <c r="L11" s="3">
         <v>5</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" s="3">
+        <v>1</v>
+      </c>
+      <c r="N11" t="s">
         <v>67</v>
       </c>
-      <c r="M11" t="s">
+      <c r="O11" t="s">
         <v>68</v>
       </c>
-      <c r="N11" t="s">
+      <c r="P11" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[update] entity comment added
</commit_message>
<xml_diff>
--- a/input_glpi.xlsx
+++ b/input_glpi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OneDriveFalse\1 - KevDev\2 - Estudos\Testes de codigo\GLPI scripts\Input de informações e criação de coisas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AC6CA8-90FC-40EE-9BAD-7980FF8D22AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2497C7AB-C0CB-469E-A5B7-8968D06D7F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="116">
   <si>
     <t>Nome do User</t>
   </si>
@@ -360,6 +360,27 @@
   </si>
   <si>
     <t>Status User</t>
+  </si>
+  <si>
+    <t>Dimensões</t>
+  </si>
+  <si>
+    <t>Teste</t>
+  </si>
+  <si>
+    <t>BS123|32131|WD1</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>BBBB</t>
+  </si>
+  <si>
+    <t>SFADSAD</t>
+  </si>
+  <si>
+    <t>AAAAA</t>
   </si>
 </sst>
 </file>
@@ -725,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:AA11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,24 +760,25 @@
     <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.42578125" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1"/>
-    <col min="11" max="13" width="13.140625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="13.140625" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" style="3" customWidth="1"/>
-    <col min="18" max="18" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20" customWidth="1"/>
-    <col min="20" max="20" width="27" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20" customWidth="1"/>
-    <col min="23" max="23" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1"/>
+    <col min="12" max="14" width="13.140625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.140625" style="3" customWidth="1"/>
+    <col min="19" max="19" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20" customWidth="1"/>
+    <col min="21" max="21" width="27" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20" customWidth="1"/>
+    <col min="24" max="24" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -781,62 +803,65 @@
       <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -858,62 +883,65 @@
       <c r="G2" t="s">
         <v>84</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>81</v>
       </c>
-      <c r="K2" s="3">
-        <v>1</v>
-      </c>
       <c r="L2" s="3">
+        <v>1</v>
+      </c>
+      <c r="M2" s="3">
         <v>3</v>
       </c>
-      <c r="M2" s="3">
-        <v>1</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="N2" s="3">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
         <v>64</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>11</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>13</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>58</v>
       </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2" t="s">
         <v>14</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>74</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>94</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>97</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>100</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -935,35 +963,38 @@
       <c r="G3" t="s">
         <v>84</v>
       </c>
-      <c r="R3" t="s">
+      <c r="I3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="S3" t="s">
         <v>16</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>59</v>
       </c>
-      <c r="T3">
-        <v>1</v>
-      </c>
-      <c r="U3" t="s">
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3" t="s">
         <v>17</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>75</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="X3" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="Z3" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="Z3" s="3" t="s">
+      <c r="AA3" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -988,60 +1019,63 @@
       <c r="H4" t="s">
         <v>86</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="J4" t="s">
         <v>19</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>82</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L4" s="3">
         <v>2</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="3">
         <v>3</v>
       </c>
-      <c r="M4" s="3">
+      <c r="N4" s="3">
         <v>2</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>65</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>70</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>20</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>21</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>60</v>
       </c>
-      <c r="T4">
-        <v>1</v>
-      </c>
-      <c r="U4" t="s">
+      <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4" t="s">
         <v>22</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>76</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>95</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="Z4" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -1063,9 +1097,12 @@
       <c r="H5" t="s">
         <v>87</v>
       </c>
-      <c r="Z5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA5" s="3"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1090,33 +1127,36 @@
       <c r="H6" t="s">
         <v>86</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="J6" t="s">
         <v>25</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>82</v>
       </c>
-      <c r="K6" s="3">
-        <v>1</v>
-      </c>
       <c r="L6" s="3">
+        <v>1</v>
+      </c>
+      <c r="M6" s="3">
         <v>3</v>
       </c>
-      <c r="M6" s="3">
-        <v>1</v>
-      </c>
-      <c r="N6" t="s">
+      <c r="N6" s="3">
+        <v>1</v>
+      </c>
+      <c r="O6" t="s">
         <v>66</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>69</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>26</v>
       </c>
-      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1135,35 +1175,38 @@
       <c r="G7" t="s">
         <v>89</v>
       </c>
-      <c r="R7" t="s">
+      <c r="I7" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="S7" t="s">
         <v>13</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>61</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>2</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>28</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>77</v>
       </c>
-      <c r="W7" s="3" t="s">
+      <c r="X7" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>98</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
         <v>99</v>
       </c>
-      <c r="Z7" s="3" t="s">
+      <c r="AA7" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1185,33 +1228,36 @@
       <c r="G8" t="s">
         <v>65</v>
       </c>
-      <c r="R8" t="s">
+      <c r="I8" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="S8" t="s">
         <v>30</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>62</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>2</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>31</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>78</v>
       </c>
-      <c r="W8" s="3" t="s">
+      <c r="X8" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="X8" s="3" t="s">
+      <c r="Y8" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="Y8" s="3" t="s">
+      <c r="Z8" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1230,33 +1276,36 @@
       <c r="G9" t="s">
         <v>65</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="J9" t="s">
         <v>33</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>82</v>
       </c>
-      <c r="K9" s="3">
+      <c r="L9" s="3">
         <v>2</v>
       </c>
-      <c r="L9" s="3">
+      <c r="M9" s="3">
         <v>5</v>
       </c>
-      <c r="M9" s="3">
-        <v>1</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="N9" s="3">
+        <v>1</v>
+      </c>
+      <c r="O9" t="s">
         <v>64</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>34</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>35</v>
       </c>
-      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1278,33 +1327,36 @@
       <c r="G10" t="s">
         <v>37</v>
       </c>
-      <c r="R10" t="s">
+      <c r="I10" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="S10" t="s">
         <v>16</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>63</v>
       </c>
-      <c r="T10">
-        <v>1</v>
-      </c>
-      <c r="U10" t="s">
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10" t="s">
         <v>38</v>
       </c>
-      <c r="V10" t="s">
+      <c r="W10" t="s">
         <v>79</v>
       </c>
-      <c r="W10" s="3" t="s">
+      <c r="X10" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="X10" s="3" t="s">
+      <c r="Y10" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="Z10" t="s">
         <v>99</v>
       </c>
-      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1326,28 +1378,31 @@
       <c r="G11" t="s">
         <v>88</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J11" t="s">
         <v>40</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>81</v>
       </c>
-      <c r="K11" s="3">
+      <c r="L11" s="3">
         <v>3</v>
       </c>
-      <c r="L11" s="3">
+      <c r="M11" s="3">
         <v>5</v>
       </c>
-      <c r="M11" s="3">
-        <v>1</v>
-      </c>
-      <c r="N11" t="s">
+      <c r="N11" s="3">
+        <v>1</v>
+      </c>
+      <c r="O11" t="s">
         <v>67</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>68</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[feature] manufactor and contracts added in lines and notes
</commit_message>
<xml_diff>
--- a/input_glpi.xlsx
+++ b/input_glpi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OneDriveFalse\1 - KevDev\2 - Estudos\Testes de codigo\GLPI scripts\Input de informações e criação de coisas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2497C7AB-C0CB-469E-A5B7-8968D06D7F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D42261-549E-423C-858E-1CD1B843171D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="132">
   <si>
     <t>Nome do User</t>
   </si>
@@ -131,9 +131,6 @@
     <t>ACR12345</t>
   </si>
   <si>
-    <t>Fernanda Lima</t>
-  </si>
-  <si>
     <t>551196666555</t>
   </si>
   <si>
@@ -191,9 +188,6 @@
     <t>Ra@email.com</t>
   </si>
   <si>
-    <t>Fe@email.com</t>
-  </si>
-  <si>
     <t>Br@email.com</t>
   </si>
   <si>
@@ -338,12 +332,6 @@
     <t>8GB</t>
   </si>
   <si>
-    <t>Plano</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Tipo de celular</t>
   </si>
   <si>
@@ -381,13 +369,76 @@
   </si>
   <si>
     <t>AAAAA</t>
+  </si>
+  <si>
+    <t>Status linha</t>
+  </si>
+  <si>
+    <t>tipo de linha</t>
+  </si>
+  <si>
+    <t>data inicial linha</t>
+  </si>
+  <si>
+    <t>valor linha</t>
+  </si>
+  <si>
+    <t>contrato notebook</t>
+  </si>
+  <si>
+    <t>Comprado em Notebook</t>
+  </si>
+  <si>
+    <t>Fornecedor Notebook</t>
+  </si>
+  <si>
+    <t>Weback</t>
+  </si>
+  <si>
+    <t>Agasus</t>
+  </si>
+  <si>
+    <t>GI</t>
+  </si>
+  <si>
+    <t>Fornecedor Linha</t>
+  </si>
+  <si>
+    <t>TIM S.A</t>
+  </si>
+  <si>
+    <t>VIVO</t>
+  </si>
+  <si>
+    <t>Contrato Linha</t>
+  </si>
+  <si>
+    <t>Estoque</t>
+  </si>
+  <si>
+    <t>Gestão de ativos</t>
+  </si>
+  <si>
+    <t>C2C584312</t>
+  </si>
+  <si>
+    <t>HPPB450-204</t>
+  </si>
+  <si>
+    <t>Status Notebook</t>
+  </si>
+  <si>
+    <t>Status celular</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,6 +456,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -433,19 +491,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Moeda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -746,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA11"/>
+  <dimension ref="A1:AJ14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,33 +826,34 @@
     <col min="9" max="9" width="10.42578125" style="3" customWidth="1"/>
     <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.140625" customWidth="1"/>
-    <col min="12" max="14" width="13.140625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" customWidth="1"/>
-    <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.140625" style="3" customWidth="1"/>
-    <col min="19" max="19" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20" customWidth="1"/>
-    <col min="21" max="21" width="27" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20" customWidth="1"/>
-    <col min="24" max="24" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="18" width="13.140625" style="3" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" customWidth="1"/>
+    <col min="20" max="20" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="16.140625" style="3" customWidth="1"/>
+    <col min="24" max="24" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20" customWidth="1"/>
+    <col min="26" max="26" width="27" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20" customWidth="1"/>
+    <col min="29" max="29" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="34" width="23.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -804,69 +868,96 @@
         <v>3</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="M1" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AI1" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="N1" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="AA1" s="4" t="s">
-        <v>106</v>
+      <c r="AJ1" s="4" t="s">
+        <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2">
         <v>35686234657</v>
@@ -875,25 +966,25 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="J2" t="s">
         <v>10</v>
       </c>
       <c r="K2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L2" s="3">
-        <v>1</v>
+        <v>1432131</v>
       </c>
       <c r="M2" s="3">
         <v>3</v>
@@ -901,52 +992,79 @@
       <c r="N2" s="3">
         <v>1</v>
       </c>
-      <c r="O2" t="s">
-        <v>64</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="O2" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="P2" s="5">
+        <v>44816</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>34.9</v>
+      </c>
+      <c r="R2" s="3">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
+        <v>62</v>
+      </c>
+      <c r="T2" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="U2" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="V2" s="3">
+        <v>10</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="X2" t="s">
         <v>13</v>
       </c>
-      <c r="T2" t="s">
-        <v>58</v>
-      </c>
-      <c r="U2">
-        <v>1</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="Y2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="s">
         <v>14</v>
       </c>
-      <c r="W2" t="s">
-        <v>74</v>
-      </c>
-      <c r="X2" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>97</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>107</v>
+      <c r="AB2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF2" s="3">
+        <v>31873187</v>
+      </c>
+      <c r="AG2" s="5">
+        <v>44816</v>
+      </c>
+      <c r="AH2" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="AJ2">
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3">
         <v>35686234658</v>
@@ -955,51 +1073,64 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="S3" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q3" s="6"/>
+      <c r="X3" t="s">
         <v>16</v>
       </c>
-      <c r="T3" t="s">
-        <v>59</v>
-      </c>
-      <c r="U3">
-        <v>1</v>
-      </c>
-      <c r="V3" t="s">
+      <c r="Y3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3" t="s">
         <v>17</v>
       </c>
-      <c r="W3" t="s">
-        <v>75</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y3" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="Z3" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>107</v>
+      <c r="AB3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AF3" s="3">
+        <v>371871378</v>
+      </c>
+      <c r="AG3" s="5">
+        <v>44816</v>
+      </c>
+      <c r="AH3" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="AJ3" s="3">
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4">
         <v>35686234659</v>
@@ -1008,28 +1139,28 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="J4" t="s">
         <v>19</v>
       </c>
       <c r="K4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L4" s="3">
-        <v>2</v>
+        <v>321421</v>
       </c>
       <c r="M4" s="3">
         <v>3</v>
@@ -1037,77 +1168,105 @@
       <c r="N4" s="3">
         <v>2</v>
       </c>
-      <c r="O4" t="s">
-        <v>65</v>
-      </c>
-      <c r="P4" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="O4" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="P4" s="5">
+        <v>44816</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>34.9</v>
+      </c>
+      <c r="R4" s="3">
+        <v>2</v>
+      </c>
+      <c r="S4" t="s">
+        <v>63</v>
+      </c>
+      <c r="T4" t="s">
+        <v>68</v>
+      </c>
+      <c r="U4" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="S4" t="s">
+      <c r="V4" s="3">
+        <v>10</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="X4" t="s">
         <v>21</v>
       </c>
-      <c r="T4" t="s">
-        <v>60</v>
-      </c>
-      <c r="U4">
-        <v>1</v>
-      </c>
-      <c r="V4" t="s">
+      <c r="Y4" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z4">
+        <v>1</v>
+      </c>
+      <c r="AA4" t="s">
         <v>22</v>
       </c>
-      <c r="W4" t="s">
-        <v>76</v>
-      </c>
-      <c r="X4" t="s">
+      <c r="AB4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD4" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="AE4" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="Z4" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="AA4" s="3"/>
+      <c r="AF4" s="3">
+        <v>8137831</v>
+      </c>
+      <c r="AG4" s="5">
+        <v>44816</v>
+      </c>
+      <c r="AH4" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI4" s="3"/>
+      <c r="AJ4" s="3">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="3">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G5" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" t="s">
         <v>85</v>
       </c>
-      <c r="H5" t="s">
-        <v>87</v>
-      </c>
       <c r="I5" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="AA5" s="3"/>
+        <v>107</v>
+      </c>
+      <c r="Q5" s="6"/>
+      <c r="AI5" s="3"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6">
         <v>35686234661</v>
@@ -1116,28 +1275,28 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="J6" t="s">
         <v>25</v>
       </c>
       <c r="K6" t="s">
-        <v>82</v>
-      </c>
-      <c r="L6" s="3">
-        <v>1</v>
+        <v>80</v>
+      </c>
+      <c r="L6" s="7">
+        <v>51231233</v>
       </c>
       <c r="M6" s="3">
         <v>3</v>
@@ -1145,73 +1304,101 @@
       <c r="N6" s="3">
         <v>1</v>
       </c>
-      <c r="O6" t="s">
-        <v>66</v>
-      </c>
-      <c r="P6" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q6" t="s">
+      <c r="O6" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="P6" s="5">
+        <v>44816</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>34.9</v>
+      </c>
+      <c r="R6" s="3">
+        <v>1</v>
+      </c>
+      <c r="S6" t="s">
+        <v>64</v>
+      </c>
+      <c r="T6" t="s">
+        <v>67</v>
+      </c>
+      <c r="U6" t="s">
         <v>26</v>
       </c>
-      <c r="AA6" s="3"/>
+      <c r="V6" s="3">
+        <v>10</v>
+      </c>
+      <c r="AI6" s="3"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="3">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="S7" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q7" s="6"/>
+      <c r="X7" t="s">
         <v>13</v>
       </c>
-      <c r="T7" t="s">
-        <v>61</v>
-      </c>
-      <c r="U7">
+      <c r="Y7" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z7">
         <v>2</v>
       </c>
-      <c r="V7" t="s">
+      <c r="AA7" t="s">
         <v>28</v>
       </c>
-      <c r="W7" t="s">
-        <v>77</v>
-      </c>
-      <c r="X7" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>99</v>
-      </c>
-      <c r="AA7" s="3" t="s">
-        <v>105</v>
+      <c r="AB7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC7" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>96</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>97</v>
+      </c>
+      <c r="AF7" s="3">
+        <v>31781387</v>
+      </c>
+      <c r="AG7" s="5">
+        <v>44816</v>
+      </c>
+      <c r="AH7" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI7" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AJ7" s="3">
+        <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8">
         <v>35686234663</v>
@@ -1220,196 +1407,323 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="S8" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q8" s="6"/>
+      <c r="X8" t="s">
         <v>30</v>
       </c>
-      <c r="T8" t="s">
-        <v>62</v>
-      </c>
-      <c r="U8">
+      <c r="Y8" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z8">
         <v>2</v>
       </c>
-      <c r="V8" t="s">
+      <c r="AA8" t="s">
         <v>31</v>
       </c>
-      <c r="W8" t="s">
-        <v>78</v>
-      </c>
-      <c r="X8" s="3" t="s">
+      <c r="AB8" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC8" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AD8" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="Y8" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z8" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="AA8" s="3"/>
+      <c r="AE8" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AF8" s="3">
+        <v>317871378</v>
+      </c>
+      <c r="AG8" s="5">
+        <v>44816</v>
+      </c>
+      <c r="AH8" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI8" s="3"/>
+      <c r="AJ8" s="3">
+        <v>8</v>
+      </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" t="s">
+        <v>127</v>
+      </c>
+      <c r="H9" t="s">
+        <v>126</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="J9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D9" s="3">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" t="s">
-        <v>65</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="J9" t="s">
-        <v>33</v>
-      </c>
       <c r="K9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L9" s="3">
-        <v>2</v>
+        <v>321421</v>
       </c>
       <c r="M9" s="3">
         <v>5</v>
       </c>
       <c r="N9" s="3">
-        <v>1</v>
-      </c>
-      <c r="O9" t="s">
-        <v>64</v>
-      </c>
-      <c r="P9" t="s">
+        <v>2</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="P9" s="5">
+        <v>44816</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>34.9</v>
+      </c>
+      <c r="AI9" s="3"/>
+    </row>
+    <row r="10" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="3">
+        <v>1</v>
+      </c>
+      <c r="S10" t="s">
+        <v>62</v>
+      </c>
+      <c r="T10" t="s">
+        <v>33</v>
+      </c>
+      <c r="U10" t="s">
         <v>34</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="V10" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="6"/>
+      <c r="X11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="AB11" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="AC11" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD11" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AE11" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AF11" s="3">
+        <v>31989139</v>
+      </c>
+      <c r="AG11" s="5">
+        <v>44816</v>
+      </c>
+      <c r="AH11" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="AJ11" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>35</v>
       </c>
-      <c r="AA9" s="3"/>
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12">
+        <v>35686234665</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q12" s="6"/>
+      <c r="X12" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z12">
+        <v>1</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC12" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AD12" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>97</v>
+      </c>
+      <c r="AF12" s="3">
+        <v>31989139</v>
+      </c>
+      <c r="AG12" s="5">
+        <v>44816</v>
+      </c>
+      <c r="AH12" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="AI12" s="3"/>
+      <c r="AJ12" s="3">
+        <v>8</v>
+      </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10">
-        <v>35686234665</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" t="s">
-        <v>57</v>
-      </c>
-      <c r="G10" t="s">
-        <v>37</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="S10" t="s">
-        <v>16</v>
-      </c>
-      <c r="T10" t="s">
-        <v>63</v>
-      </c>
-      <c r="U10">
-        <v>1</v>
-      </c>
-      <c r="V10" t="s">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>38</v>
       </c>
-      <c r="W10" t="s">
+      <c r="B13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13">
+        <v>35686234666</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" t="s">
+        <v>86</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J13" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" t="s">
         <v>79</v>
       </c>
-      <c r="X10" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="Y10" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>99</v>
-      </c>
-      <c r="AA10" s="3"/>
+      <c r="L13" s="3">
+        <v>1432131</v>
+      </c>
+      <c r="M13" s="3">
+        <v>5</v>
+      </c>
+      <c r="N13" s="3">
+        <v>3</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="P13" s="5">
+        <v>44816</v>
+      </c>
+      <c r="Q13" s="6">
+        <v>34.9</v>
+      </c>
+      <c r="R13" s="3">
+        <v>1</v>
+      </c>
+      <c r="S13" t="s">
+        <v>65</v>
+      </c>
+      <c r="T13" t="s">
+        <v>66</v>
+      </c>
+      <c r="U13" t="s">
+        <v>40</v>
+      </c>
+      <c r="V13" s="3">
+        <v>10</v>
+      </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11">
-        <v>35686234666</v>
-      </c>
-      <c r="D11" s="3">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" t="s">
-        <v>88</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="J11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K11" t="s">
-        <v>81</v>
-      </c>
-      <c r="L11" s="3">
-        <v>3</v>
-      </c>
-      <c r="M11" s="3">
-        <v>5</v>
-      </c>
-      <c r="N11" s="3">
-        <v>1</v>
-      </c>
-      <c r="O11" t="s">
-        <v>67</v>
-      </c>
-      <c r="P11" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>41</v>
-      </c>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="P14" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1" xr:uid="{A666A66F-87FA-46AB-96C6-68D6501B3CE2}"/>
+    <hyperlink ref="B13" r:id="rId1" xr:uid="{A666A66F-87FA-46AB-96C6-68D6501B3CE2}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>